<commit_message>
fix docker-compose and update init files
</commit_message>
<xml_diff>
--- a/backend/db_init/db_sign.xlsx
+++ b/backend/db_init/db_sign.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinyuntae/docker_volume/passionpayweb/backend/db_init/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F62DA57B-52F8-A743-99A4-776E4B653A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F300AE8-231C-F444-97A7-AA79FAA750FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5040" yWindow="1800" windowWidth="28300" windowHeight="17440" xr2:uid="{74AD0C59-56FF-6B48-9434-BD12CA846D85}"/>
   </bookViews>
@@ -58,7 +58,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hello1</t>
+    <t>hello_user</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>